<commit_message>
- add storage heating and shapes from HES for elec heating - dummy transport model
</commit_message>
<xml_diff>
--- a/data/submodel_residential/_EXCELFILES/SANSOM_residential_gas_hourly_shape.xlsx
+++ b/data/submodel_residential/_EXCELFILES/SANSOM_residential_gas_hourly_shape.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="390" windowWidth="27555" windowHeight="12315" activeTab="1"/>
+    <workbookView xWindow="720" yWindow="450" windowWidth="27555" windowHeight="12255" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -16,10 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
-  <si>
-    <t>Day</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>Wkday</t>
   </si>
@@ -126,7 +123,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>original!$B$10:$Y$10</c:f>
+              <c:f>original!$B$9:$Y$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
@@ -215,7 +212,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>original!$B$11:$Y$11</c:f>
+              <c:f>original!$B$10:$Y$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
@@ -304,7 +301,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>original!$B$23:$Y$23</c:f>
+              <c:f>original!$B$21:$Y$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
@@ -395,11 +392,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="84017536"/>
-        <c:axId val="84019072"/>
+        <c:axId val="153789952"/>
+        <c:axId val="153791488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="84017536"/>
+        <c:axId val="153789952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -408,7 +405,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84019072"/>
+        <c:crossAx val="153791488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -416,7 +413,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84019072"/>
+        <c:axId val="153791488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -427,7 +424,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84017536"/>
+        <c:crossAx val="153789952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -524,13 +521,13 @@
     <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -616,13 +613,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>179205</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -671,13 +668,13 @@
     <xdr:from>
       <xdr:col>24</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>108857</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>39</xdr:col>
       <xdr:colOff>394611</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>149680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -990,7 +987,7 @@
   <dimension ref="A1:X5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1373,10 +1370,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AW24"/>
+  <dimension ref="A2:AW22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AA23" sqref="AA23"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1533,12 +1530,12 @@
     </row>
     <row r="6" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:49" x14ac:dyDescent="0.25">
@@ -1615,7 +1612,7 @@
         <v>23</v>
       </c>
       <c r="Z8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:49" x14ac:dyDescent="0.25">
@@ -1638,34 +1635,34 @@
         <v>0.2</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H9">
-        <v>2.2999999999999998</v>
+        <v>3</v>
       </c>
       <c r="I9">
-        <v>3.9</v>
+        <v>4.8</v>
       </c>
       <c r="J9">
-        <v>2.8</v>
+        <v>2.6</v>
       </c>
       <c r="K9">
-        <v>1.5</v>
+        <v>1.2</v>
       </c>
       <c r="L9">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="M9">
+        <v>1.3</v>
+      </c>
+      <c r="N9">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O9">
         <v>1.2</v>
       </c>
-      <c r="M9">
-        <v>1.5</v>
-      </c>
-      <c r="N9">
-        <v>1.3</v>
-      </c>
-      <c r="O9">
-        <v>1.3</v>
-      </c>
       <c r="P9">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="Q9">
         <v>2</v>
@@ -1680,7 +1677,7 @@
         <v>4.7</v>
       </c>
       <c r="U9">
-        <v>3.8</v>
+        <v>3.9</v>
       </c>
       <c r="V9">
         <v>3.1</v>
@@ -1695,8 +1692,8 @@
         <v>0.5</v>
       </c>
       <c r="Z9">
-        <f>SUM(B9:Y9)</f>
-        <v>45.8</v>
+        <f t="shared" ref="Z9:Z10" si="0">SUM(B9:Y9)</f>
+        <v>46.4</v>
       </c>
     </row>
     <row r="10" spans="1:49" x14ac:dyDescent="0.25">
@@ -1719,40 +1716,40 @@
         <v>0.2</v>
       </c>
       <c r="G10">
-        <v>1.1000000000000001</v>
+        <v>0.6</v>
       </c>
       <c r="H10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I10">
-        <v>4.8</v>
+        <v>2.5</v>
       </c>
       <c r="J10">
-        <v>2.6</v>
+        <v>4.5</v>
       </c>
       <c r="K10">
-        <v>1.2</v>
+        <v>2.5</v>
       </c>
       <c r="L10">
-        <v>1.1000000000000001</v>
+        <v>1.5</v>
       </c>
       <c r="M10">
-        <v>1.3</v>
+        <v>1.6</v>
       </c>
       <c r="N10">
-        <v>1.1000000000000001</v>
+        <v>2</v>
       </c>
       <c r="O10">
-        <v>1.2</v>
+        <v>1.6</v>
       </c>
       <c r="P10">
-        <v>1.2</v>
+        <v>1.6</v>
       </c>
       <c r="Q10">
-        <v>2</v>
+        <v>2.1</v>
       </c>
       <c r="R10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S10">
         <v>4.8</v>
@@ -1761,7 +1758,7 @@
         <v>4.7</v>
       </c>
       <c r="U10">
-        <v>3.9</v>
+        <v>3.7</v>
       </c>
       <c r="V10">
         <v>3.1</v>
@@ -1776,750 +1773,564 @@
         <v>0.5</v>
       </c>
       <c r="Z10">
-        <f t="shared" ref="Z10:Z11" si="0">SUM(B10:Y10)</f>
-        <v>46.4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11">
-        <v>0.2</v>
-      </c>
-      <c r="C11">
-        <v>0.2</v>
-      </c>
-      <c r="D11">
-        <v>0.2</v>
-      </c>
-      <c r="E11">
-        <v>0.2</v>
-      </c>
-      <c r="F11">
-        <v>0.2</v>
-      </c>
-      <c r="G11">
-        <v>0.6</v>
-      </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="I11">
-        <v>2.5</v>
-      </c>
-      <c r="J11">
-        <v>4.5</v>
-      </c>
-      <c r="K11">
-        <v>2.5</v>
-      </c>
-      <c r="L11">
-        <v>1.5</v>
-      </c>
-      <c r="M11">
-        <v>1.6</v>
-      </c>
-      <c r="N11">
-        <v>2</v>
-      </c>
-      <c r="O11">
-        <v>1.6</v>
-      </c>
-      <c r="P11">
-        <v>1.6</v>
-      </c>
-      <c r="Q11">
-        <v>2.1</v>
-      </c>
-      <c r="R11">
-        <v>4</v>
-      </c>
-      <c r="S11">
-        <v>4.8</v>
-      </c>
-      <c r="T11">
-        <v>4.7</v>
-      </c>
-      <c r="U11">
-        <v>3.7</v>
-      </c>
-      <c r="V11">
-        <v>3.1</v>
-      </c>
-      <c r="W11">
-        <v>2.9</v>
-      </c>
-      <c r="X11">
-        <v>1.9</v>
-      </c>
-      <c r="Y11">
-        <v>0.5</v>
-      </c>
-      <c r="Z11">
         <f t="shared" si="0"/>
         <v>48.100000000000009</v>
       </c>
     </row>
+    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+    </row>
     <row r="14" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14">
+        <v>4</v>
+      </c>
+      <c r="G14">
         <v>5</v>
+      </c>
+      <c r="H14">
+        <v>6</v>
+      </c>
+      <c r="I14">
+        <v>7</v>
+      </c>
+      <c r="J14">
+        <v>8</v>
+      </c>
+      <c r="K14">
+        <v>9</v>
+      </c>
+      <c r="L14">
+        <v>10</v>
+      </c>
+      <c r="M14">
+        <v>11</v>
+      </c>
+      <c r="N14">
+        <v>12</v>
+      </c>
+      <c r="O14">
+        <v>13</v>
+      </c>
+      <c r="P14">
+        <v>14</v>
+      </c>
+      <c r="Q14">
+        <v>15</v>
+      </c>
+      <c r="R14">
+        <v>16</v>
+      </c>
+      <c r="S14">
+        <v>17</v>
+      </c>
+      <c r="T14">
+        <v>18</v>
+      </c>
+      <c r="U14">
+        <v>19</v>
+      </c>
+      <c r="V14">
+        <v>20</v>
+      </c>
+      <c r="W14">
+        <v>21</v>
+      </c>
+      <c r="X14">
+        <v>22</v>
+      </c>
+      <c r="Y14">
+        <v>23</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
       <c r="B15">
-        <v>0</v>
+        <f>(100/$Z9)*B9</f>
+        <v>0.43103448275862077</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <f>(100/$Z9)*C9</f>
+        <v>0.43103448275862077</v>
       </c>
       <c r="D15">
-        <v>2</v>
+        <f>(100/$Z9)*D9</f>
+        <v>0.43103448275862077</v>
       </c>
       <c r="E15">
-        <v>3</v>
+        <f>(100/$Z9)*E9</f>
+        <v>0.43103448275862077</v>
       </c>
       <c r="F15">
-        <v>4</v>
+        <f>(100/$Z9)*F9</f>
+        <v>0.43103448275862077</v>
       </c>
       <c r="G15">
-        <v>5</v>
+        <f>(100/$Z9)*G9</f>
+        <v>2.3706896551724141</v>
       </c>
       <c r="H15">
-        <v>6</v>
+        <f>(100/$Z9)*H9</f>
+        <v>6.4655172413793114</v>
       </c>
       <c r="I15">
-        <v>7</v>
+        <f>(100/$Z9)*I9</f>
+        <v>10.344827586206897</v>
       </c>
       <c r="J15">
-        <v>8</v>
+        <f>(100/$Z9)*J9</f>
+        <v>5.6034482758620694</v>
       </c>
       <c r="K15">
-        <v>9</v>
+        <f>(100/$Z9)*K9</f>
+        <v>2.5862068965517242</v>
       </c>
       <c r="L15">
-        <v>10</v>
+        <f>(100/$Z9)*L9</f>
+        <v>2.3706896551724141</v>
       </c>
       <c r="M15">
-        <v>11</v>
+        <f>(100/$Z9)*M9</f>
+        <v>2.8017241379310347</v>
       </c>
       <c r="N15">
-        <v>12</v>
+        <f>(100/$Z9)*N9</f>
+        <v>2.3706896551724141</v>
       </c>
       <c r="O15">
-        <v>13</v>
+        <f>(100/$Z9)*O9</f>
+        <v>2.5862068965517242</v>
       </c>
       <c r="P15">
-        <v>14</v>
+        <f>(100/$Z9)*P9</f>
+        <v>2.5862068965517242</v>
       </c>
       <c r="Q15">
-        <v>15</v>
+        <f>(100/$Z9)*Q9</f>
+        <v>4.3103448275862073</v>
       </c>
       <c r="R15">
-        <v>16</v>
+        <f>(100/$Z9)*R9</f>
+        <v>6.4655172413793114</v>
       </c>
       <c r="S15">
-        <v>17</v>
+        <f>(100/$Z9)*S9</f>
+        <v>10.344827586206897</v>
       </c>
       <c r="T15">
-        <v>18</v>
+        <f>(100/$Z9)*T9</f>
+        <v>10.129310344827587</v>
       </c>
       <c r="U15">
-        <v>19</v>
+        <f>(100/$Z9)*U9</f>
+        <v>8.4051724137931032</v>
       </c>
       <c r="V15">
-        <v>20</v>
+        <f>(100/$Z9)*V9</f>
+        <v>6.6810344827586219</v>
       </c>
       <c r="W15">
-        <v>21</v>
+        <f>(100/$Z9)*W9</f>
+        <v>6.25</v>
       </c>
       <c r="X15">
-        <v>22</v>
+        <f>(100/$Z9)*X9</f>
+        <v>4.0948275862068968</v>
       </c>
       <c r="Y15">
-        <v>23</v>
-      </c>
-      <c r="Z15" t="s">
-        <v>4</v>
+        <f>(100/$Z9)*Y9</f>
+        <v>1.0775862068965518</v>
+      </c>
+      <c r="Z15">
+        <f>SUM(B15:Y15)</f>
+        <v>100.00000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B16">
-        <f>(100/$Z9)*B9</f>
-        <v>0.43668122270742366</v>
+        <f>(100/$Z10)*B10</f>
+        <v>0.41580041580041577</v>
       </c>
       <c r="C16">
-        <f t="shared" ref="C16:Y16" si="1">(100/$Z9)*C9</f>
-        <v>0.43668122270742366</v>
+        <f>(100/$Z10)*C10</f>
+        <v>0.41580041580041577</v>
       </c>
       <c r="D16">
-        <f t="shared" si="1"/>
-        <v>0.43668122270742366</v>
+        <f>(100/$Z10)*D10</f>
+        <v>0.41580041580041577</v>
       </c>
       <c r="E16">
-        <f t="shared" si="1"/>
-        <v>0.43668122270742366</v>
+        <f>(100/$Z10)*E10</f>
+        <v>0.41580041580041577</v>
       </c>
       <c r="F16">
-        <f t="shared" si="1"/>
-        <v>0.43668122270742366</v>
+        <f>(100/$Z10)*F10</f>
+        <v>0.41580041580041577</v>
       </c>
       <c r="G16">
-        <f t="shared" si="1"/>
-        <v>2.1834061135371181</v>
+        <f>(100/$Z10)*G10</f>
+        <v>1.2474012474012472</v>
       </c>
       <c r="H16">
-        <f t="shared" si="1"/>
-        <v>5.0218340611353716</v>
+        <f>(100/$Z10)*H10</f>
+        <v>2.0790020790020787</v>
       </c>
       <c r="I16">
-        <f t="shared" si="1"/>
-        <v>8.5152838427947604</v>
+        <f>(100/$Z10)*I10</f>
+        <v>5.1975051975051967</v>
       </c>
       <c r="J16">
-        <f t="shared" si="1"/>
-        <v>6.1135371179039302</v>
+        <f>(100/$Z10)*J10</f>
+        <v>9.3555093555093549</v>
       </c>
       <c r="K16">
-        <f t="shared" si="1"/>
-        <v>3.2751091703056772</v>
+        <f>(100/$Z10)*K10</f>
+        <v>5.1975051975051967</v>
       </c>
       <c r="L16">
-        <f t="shared" si="1"/>
-        <v>2.6200873362445418</v>
+        <f>(100/$Z10)*L10</f>
+        <v>3.118503118503118</v>
       </c>
       <c r="M16">
-        <f t="shared" si="1"/>
-        <v>3.2751091703056772</v>
+        <f>(100/$Z10)*M10</f>
+        <v>3.3264033264033261</v>
       </c>
       <c r="N16">
-        <f t="shared" si="1"/>
-        <v>2.8384279475982535</v>
+        <f>(100/$Z10)*N10</f>
+        <v>4.1580041580041573</v>
       </c>
       <c r="O16">
-        <f t="shared" si="1"/>
-        <v>2.8384279475982535</v>
+        <f>(100/$Z10)*O10</f>
+        <v>3.3264033264033261</v>
       </c>
       <c r="P16">
-        <f t="shared" si="1"/>
-        <v>2.8384279475982535</v>
+        <f>(100/$Z10)*P10</f>
+        <v>3.3264033264033261</v>
       </c>
       <c r="Q16">
-        <f t="shared" si="1"/>
-        <v>4.3668122270742362</v>
+        <f>(100/$Z10)*Q10</f>
+        <v>4.365904365904365</v>
       </c>
       <c r="R16">
-        <f t="shared" si="1"/>
-        <v>6.5502183406113543</v>
+        <f>(100/$Z10)*R10</f>
+        <v>8.3160083160083147</v>
       </c>
       <c r="S16">
-        <f t="shared" si="1"/>
-        <v>10.480349344978167</v>
+        <f>(100/$Z10)*S10</f>
+        <v>9.979209979209978</v>
       </c>
       <c r="T16">
-        <f t="shared" si="1"/>
-        <v>10.262008733624455</v>
+        <f>(100/$Z10)*T10</f>
+        <v>9.7713097713097703</v>
       </c>
       <c r="U16">
-        <f t="shared" si="1"/>
-        <v>8.2969432314410483</v>
+        <f>(100/$Z10)*U10</f>
+        <v>7.6923076923076916</v>
       </c>
       <c r="V16">
-        <f t="shared" si="1"/>
-        <v>6.7685589519650664</v>
+        <f>(100/$Z10)*V10</f>
+        <v>6.4449064449064437</v>
       </c>
       <c r="W16">
-        <f t="shared" si="1"/>
-        <v>6.3318777292576423</v>
+        <f>(100/$Z10)*W10</f>
+        <v>6.0291060291060283</v>
       </c>
       <c r="X16">
-        <f t="shared" si="1"/>
-        <v>4.1484716157205241</v>
+        <f>(100/$Z10)*X10</f>
+        <v>3.9501039501039492</v>
       </c>
       <c r="Y16">
-        <f t="shared" si="1"/>
-        <v>1.0917030567685591</v>
+        <f>(100/$Z10)*Y10</f>
+        <v>1.0395010395010393</v>
       </c>
       <c r="Z16">
         <f>SUM(B16:Y16)</f>
-        <v>100.00000000000001</v>
+        <v>99.999999999999986</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
         <v>1</v>
       </c>
-      <c r="B17">
-        <f>(100/$Z10)*B10</f>
-        <v>0.43103448275862077</v>
-      </c>
-      <c r="C17">
-        <f t="shared" ref="C17:Y17" si="2">(100/$Z10)*C10</f>
-        <v>0.43103448275862077</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="2"/>
-        <v>0.43103448275862077</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="2"/>
-        <v>0.43103448275862077</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="2"/>
-        <v>0.43103448275862077</v>
-      </c>
-      <c r="G17">
-        <f t="shared" si="2"/>
-        <v>2.3706896551724141</v>
-      </c>
-      <c r="H17">
-        <f t="shared" si="2"/>
-        <v>6.4655172413793114</v>
-      </c>
-      <c r="I17">
-        <f t="shared" si="2"/>
-        <v>10.344827586206897</v>
-      </c>
-      <c r="J17">
-        <f t="shared" si="2"/>
-        <v>5.6034482758620694</v>
-      </c>
-      <c r="K17">
-        <f t="shared" si="2"/>
-        <v>2.5862068965517242</v>
-      </c>
-      <c r="L17">
-        <f t="shared" si="2"/>
-        <v>2.3706896551724141</v>
-      </c>
-      <c r="M17">
-        <f t="shared" si="2"/>
-        <v>2.8017241379310347</v>
-      </c>
-      <c r="N17">
-        <f t="shared" si="2"/>
-        <v>2.3706896551724141</v>
-      </c>
-      <c r="O17">
-        <f t="shared" si="2"/>
-        <v>2.5862068965517242</v>
-      </c>
-      <c r="P17">
-        <f t="shared" si="2"/>
-        <v>2.5862068965517242</v>
-      </c>
-      <c r="Q17">
-        <f t="shared" si="2"/>
-        <v>4.3103448275862073</v>
-      </c>
-      <c r="R17">
-        <f t="shared" si="2"/>
-        <v>6.4655172413793114</v>
-      </c>
-      <c r="S17">
-        <f t="shared" si="2"/>
-        <v>10.344827586206897</v>
-      </c>
-      <c r="T17">
-        <f t="shared" si="2"/>
-        <v>10.129310344827587</v>
-      </c>
-      <c r="U17">
-        <f t="shared" si="2"/>
-        <v>8.4051724137931032</v>
-      </c>
-      <c r="V17">
-        <f t="shared" si="2"/>
-        <v>6.6810344827586219</v>
-      </c>
-      <c r="W17">
-        <f t="shared" si="2"/>
-        <v>6.25</v>
-      </c>
-      <c r="X17">
-        <f t="shared" si="2"/>
-        <v>4.0948275862068968</v>
-      </c>
-      <c r="Y17">
-        <f t="shared" si="2"/>
-        <v>1.0775862068965518</v>
-      </c>
-      <c r="Z17">
-        <f>SUM(B17:Y17)</f>
-        <v>100.00000000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="D20">
         <v>2</v>
       </c>
-      <c r="B18">
-        <f>(100/$Z11)*B11</f>
-        <v>0.41580041580041577</v>
-      </c>
-      <c r="C18">
-        <f t="shared" ref="C18:Y18" si="3">(100/$Z11)*C11</f>
-        <v>0.41580041580041577</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="3"/>
-        <v>0.41580041580041577</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="3"/>
-        <v>0.41580041580041577</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="3"/>
-        <v>0.41580041580041577</v>
-      </c>
-      <c r="G18">
-        <f t="shared" si="3"/>
-        <v>1.2474012474012472</v>
-      </c>
-      <c r="H18">
-        <f t="shared" si="3"/>
-        <v>2.0790020790020787</v>
-      </c>
-      <c r="I18">
-        <f t="shared" si="3"/>
-        <v>5.1975051975051967</v>
-      </c>
-      <c r="J18">
-        <f t="shared" si="3"/>
-        <v>9.3555093555093549</v>
-      </c>
-      <c r="K18">
-        <f t="shared" si="3"/>
-        <v>5.1975051975051967</v>
-      </c>
-      <c r="L18">
-        <f t="shared" si="3"/>
-        <v>3.118503118503118</v>
-      </c>
-      <c r="M18">
-        <f t="shared" si="3"/>
-        <v>3.3264033264033261</v>
-      </c>
-      <c r="N18">
-        <f t="shared" si="3"/>
-        <v>4.1580041580041573</v>
-      </c>
-      <c r="O18">
-        <f t="shared" si="3"/>
-        <v>3.3264033264033261</v>
-      </c>
-      <c r="P18">
-        <f t="shared" si="3"/>
-        <v>3.3264033264033261</v>
-      </c>
-      <c r="Q18">
-        <f t="shared" si="3"/>
-        <v>4.365904365904365</v>
-      </c>
-      <c r="R18">
-        <f t="shared" si="3"/>
-        <v>8.3160083160083147</v>
-      </c>
-      <c r="S18">
-        <f t="shared" si="3"/>
-        <v>9.979209979209978</v>
-      </c>
-      <c r="T18">
-        <f t="shared" si="3"/>
-        <v>9.7713097713097703</v>
-      </c>
-      <c r="U18">
-        <f t="shared" si="3"/>
-        <v>7.6923076923076916</v>
-      </c>
-      <c r="V18">
-        <f t="shared" si="3"/>
-        <v>6.4449064449064437</v>
-      </c>
-      <c r="W18">
-        <f t="shared" si="3"/>
-        <v>6.0291060291060283</v>
-      </c>
-      <c r="X18">
-        <f t="shared" si="3"/>
-        <v>3.9501039501039492</v>
-      </c>
-      <c r="Y18">
-        <f t="shared" si="3"/>
-        <v>1.0395010395010393</v>
-      </c>
-      <c r="Z18">
-        <f>SUM(B18:Y18)</f>
-        <v>99.999999999999986</v>
+      <c r="E20">
+        <v>3</v>
+      </c>
+      <c r="F20">
+        <v>4</v>
+      </c>
+      <c r="G20">
+        <v>5</v>
+      </c>
+      <c r="H20">
+        <v>6</v>
+      </c>
+      <c r="I20">
+        <v>7</v>
+      </c>
+      <c r="J20">
+        <v>8</v>
+      </c>
+      <c r="K20">
+        <v>9</v>
+      </c>
+      <c r="L20">
+        <v>10</v>
+      </c>
+      <c r="M20">
+        <v>11</v>
+      </c>
+      <c r="N20">
+        <v>12</v>
+      </c>
+      <c r="O20">
+        <v>13</v>
+      </c>
+      <c r="P20">
+        <v>14</v>
+      </c>
+      <c r="Q20">
+        <v>15</v>
+      </c>
+      <c r="R20">
+        <v>16</v>
+      </c>
+      <c r="S20">
+        <v>17</v>
+      </c>
+      <c r="T20">
+        <v>18</v>
+      </c>
+      <c r="U20">
+        <v>19</v>
+      </c>
+      <c r="V20">
+        <v>20</v>
+      </c>
+      <c r="W20">
+        <v>21</v>
+      </c>
+      <c r="X20">
+        <v>22</v>
+      </c>
+      <c r="Y20">
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>6</v>
       </c>
+      <c r="B21">
+        <v>0.5</v>
+      </c>
+      <c r="C21">
+        <v>0.5</v>
+      </c>
+      <c r="D21">
+        <v>0.5</v>
+      </c>
+      <c r="E21">
+        <v>0.5</v>
+      </c>
+      <c r="F21">
+        <v>1.8</v>
+      </c>
+      <c r="G21">
+        <v>2.1</v>
+      </c>
+      <c r="H21">
+        <v>4.2</v>
+      </c>
+      <c r="I21">
+        <v>6</v>
+      </c>
+      <c r="J21">
+        <v>4.8</v>
+      </c>
+      <c r="K21">
+        <v>3</v>
+      </c>
+      <c r="L21">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="M21">
+        <v>5</v>
+      </c>
+      <c r="N21">
+        <v>3.8</v>
+      </c>
+      <c r="O21">
+        <v>4</v>
+      </c>
+      <c r="P21">
+        <v>4.2</v>
+      </c>
+      <c r="Q21">
+        <v>4.7</v>
+      </c>
+      <c r="R21">
+        <v>4.3</v>
+      </c>
+      <c r="S21">
+        <v>6.6</v>
+      </c>
+      <c r="T21">
+        <v>6.8</v>
+      </c>
+      <c r="U21">
+        <v>6.5</v>
+      </c>
+      <c r="V21">
+        <v>5.9</v>
+      </c>
+      <c r="W21">
+        <v>5</v>
+      </c>
+      <c r="X21">
+        <v>2</v>
+      </c>
+      <c r="Y21">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Z21">
+        <f>SUM(B21:Y21)</f>
+        <v>88.4</v>
+      </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
       <c r="B22">
-        <v>0</v>
+        <f>100/$Z$21*B21</f>
+        <v>0.56561085972850678</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <f t="shared" ref="C22:X22" si="1">100/$Z$21*C21</f>
+        <v>0.56561085972850678</v>
       </c>
       <c r="D22">
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>0.56561085972850678</v>
       </c>
       <c r="E22">
-        <v>3</v>
+        <f t="shared" si="1"/>
+        <v>0.56561085972850678</v>
       </c>
       <c r="F22">
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>2.0361990950226243</v>
       </c>
       <c r="G22">
-        <v>5</v>
+        <f t="shared" si="1"/>
+        <v>2.3755656108597285</v>
       </c>
       <c r="H22">
-        <v>6</v>
+        <f t="shared" si="1"/>
+        <v>4.751131221719457</v>
       </c>
       <c r="I22">
-        <v>7</v>
+        <f t="shared" si="1"/>
+        <v>6.7873303167420813</v>
       </c>
       <c r="J22">
-        <v>8</v>
+        <f t="shared" si="1"/>
+        <v>5.4298642533936645</v>
       </c>
       <c r="K22">
-        <v>9</v>
+        <f t="shared" si="1"/>
+        <v>3.3936651583710407</v>
       </c>
       <c r="L22">
-        <v>10</v>
+        <f t="shared" si="1"/>
+        <v>5.2036199095022617</v>
       </c>
       <c r="M22">
-        <v>11</v>
+        <f t="shared" si="1"/>
+        <v>5.6561085972850673</v>
       </c>
       <c r="N22">
-        <v>12</v>
+        <f t="shared" si="1"/>
+        <v>4.2986425339366514</v>
       </c>
       <c r="O22">
-        <v>13</v>
+        <f t="shared" si="1"/>
+        <v>4.5248868778280542</v>
       </c>
       <c r="P22">
-        <v>14</v>
+        <f t="shared" si="1"/>
+        <v>4.751131221719457</v>
       </c>
       <c r="Q22">
-        <v>15</v>
+        <f t="shared" si="1"/>
+        <v>5.3167420814479636</v>
       </c>
       <c r="R22">
-        <v>16</v>
+        <f t="shared" si="1"/>
+        <v>4.864253393665158</v>
       </c>
       <c r="S22">
-        <v>17</v>
+        <f t="shared" si="1"/>
+        <v>7.4660633484162888</v>
       </c>
       <c r="T22">
-        <v>18</v>
+        <f t="shared" si="1"/>
+        <v>7.6923076923076916</v>
       </c>
       <c r="U22">
-        <v>19</v>
+        <f t="shared" si="1"/>
+        <v>7.3529411764705879</v>
       </c>
       <c r="V22">
-        <v>20</v>
+        <f t="shared" si="1"/>
+        <v>6.6742081447963804</v>
       </c>
       <c r="W22">
-        <v>21</v>
+        <f t="shared" si="1"/>
+        <v>5.6561085972850673</v>
       </c>
       <c r="X22">
-        <v>22</v>
+        <f t="shared" si="1"/>
+        <v>2.2624434389140271</v>
       </c>
       <c r="Y22">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23">
-        <v>0.5</v>
-      </c>
-      <c r="C23">
-        <v>0.5</v>
-      </c>
-      <c r="D23">
-        <v>0.5</v>
-      </c>
-      <c r="E23">
-        <v>0.5</v>
-      </c>
-      <c r="F23">
-        <v>1.8</v>
-      </c>
-      <c r="G23">
-        <v>2.1</v>
-      </c>
-      <c r="H23">
-        <v>4.2</v>
-      </c>
-      <c r="I23">
-        <v>6</v>
-      </c>
-      <c r="J23">
-        <v>4.8</v>
-      </c>
-      <c r="K23">
-        <v>3</v>
-      </c>
-      <c r="L23">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="M23">
-        <v>5</v>
-      </c>
-      <c r="N23">
-        <v>3.8</v>
-      </c>
-      <c r="O23">
-        <v>4</v>
-      </c>
-      <c r="P23">
-        <v>4.2</v>
-      </c>
-      <c r="Q23">
-        <v>4.7</v>
-      </c>
-      <c r="R23">
-        <v>4.3</v>
-      </c>
-      <c r="S23">
-        <v>6.6</v>
-      </c>
-      <c r="T23">
-        <v>6.8</v>
-      </c>
-      <c r="U23">
-        <v>6.5</v>
-      </c>
-      <c r="V23">
-        <v>5.9</v>
-      </c>
-      <c r="W23">
-        <v>5</v>
-      </c>
-      <c r="X23">
-        <v>2</v>
-      </c>
-      <c r="Y23">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="Z23">
-        <f>SUM(B23:Y23)</f>
-        <v>88.4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>8</v>
-      </c>
-      <c r="B24">
-        <f>100/$Z$23*B23</f>
-        <v>0.56561085972850678</v>
-      </c>
-      <c r="C24">
-        <f t="shared" ref="C24:X24" si="4">100/$Z$23*C23</f>
-        <v>0.56561085972850678</v>
-      </c>
-      <c r="D24">
-        <f t="shared" si="4"/>
-        <v>0.56561085972850678</v>
-      </c>
-      <c r="E24">
-        <f t="shared" si="4"/>
-        <v>0.56561085972850678</v>
-      </c>
-      <c r="F24">
-        <f t="shared" si="4"/>
-        <v>2.0361990950226243</v>
-      </c>
-      <c r="G24">
-        <f t="shared" si="4"/>
-        <v>2.3755656108597285</v>
-      </c>
-      <c r="H24">
-        <f t="shared" si="4"/>
-        <v>4.751131221719457</v>
-      </c>
-      <c r="I24">
-        <f t="shared" si="4"/>
-        <v>6.7873303167420813</v>
-      </c>
-      <c r="J24">
-        <f t="shared" si="4"/>
-        <v>5.4298642533936645</v>
-      </c>
-      <c r="K24">
-        <f t="shared" si="4"/>
-        <v>3.3936651583710407</v>
-      </c>
-      <c r="L24">
-        <f t="shared" si="4"/>
-        <v>5.2036199095022617</v>
-      </c>
-      <c r="M24">
-        <f t="shared" si="4"/>
-        <v>5.6561085972850673</v>
-      </c>
-      <c r="N24">
-        <f t="shared" si="4"/>
-        <v>4.2986425339366514</v>
-      </c>
-      <c r="O24">
-        <f t="shared" si="4"/>
-        <v>4.5248868778280542</v>
-      </c>
-      <c r="P24">
-        <f t="shared" si="4"/>
-        <v>4.751131221719457</v>
-      </c>
-      <c r="Q24">
-        <f t="shared" si="4"/>
-        <v>5.3167420814479636</v>
-      </c>
-      <c r="R24">
-        <f t="shared" si="4"/>
-        <v>4.864253393665158</v>
-      </c>
-      <c r="S24">
-        <f t="shared" si="4"/>
-        <v>7.4660633484162888</v>
-      </c>
-      <c r="T24">
-        <f t="shared" si="4"/>
-        <v>7.6923076923076916</v>
-      </c>
-      <c r="U24">
-        <f t="shared" si="4"/>
-        <v>7.3529411764705879</v>
-      </c>
-      <c r="V24">
-        <f t="shared" si="4"/>
-        <v>6.6742081447963804</v>
-      </c>
-      <c r="W24">
-        <f t="shared" si="4"/>
-        <v>5.6561085972850673</v>
-      </c>
-      <c r="X24">
-        <f t="shared" si="4"/>
-        <v>2.2624434389140271</v>
-      </c>
-      <c r="Y24">
-        <f>100/$Z$23*Y23</f>
+        <f>100/$Z$21*Y21</f>
         <v>1.244343891402715</v>
       </c>
-      <c r="Z24">
-        <f>SUM(B24:Y24)</f>
+      <c r="Z22">
+        <f>SUM(B22:Y22)</f>
         <v>100.00000000000001</v>
       </c>
     </row>

</xml_diff>